<commit_message>
Working to eliminated duplicates (old CAS numbers, mostly)
</commit_message>
<xml_diff>
--- a/Pirovano-2016.xlsx
+++ b/Pirovano-2016.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Net MyDocuments\PBPK papers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C191B25A-2676-4F52-9B69-4749C16D95BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -392,9 +393,6 @@
   </si>
   <si>
     <t>fenvalerate</t>
-  </si>
-  <si>
-    <t>51630-58-1</t>
   </si>
   <si>
     <t>fipronil</t>
@@ -963,11 +961,14 @@
   <si>
     <t>71751-41-2</t>
   </si>
+  <si>
+    <t>67614-33-9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.00;###0.00"/>
   </numFmts>
@@ -1423,11 +1424,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,16 +1439,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>271</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>0</v>
@@ -1464,7 +1465,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -1717,7 +1718,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>39</v>
@@ -1809,7 +1810,7 @@
         <v>46</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>35</v>
@@ -2126,7 +2127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>74</v>
       </c>
@@ -2200,7 +2201,7 @@
         <v>82</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>21</v>
@@ -2258,7 +2259,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>12</v>
@@ -2419,7 +2420,7 @@
         <v>24</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>12</v>
@@ -2453,7 +2454,7 @@
         <v>103</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>21</v>
@@ -2471,7 +2472,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>104</v>
       </c>
@@ -2485,7 +2486,7 @@
         <v>6.07</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>6</v>
@@ -2517,7 +2518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>108</v>
       </c>
@@ -2614,7 +2615,7 @@
         <v>117</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>118</v>
+        <v>282</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>4</v>
@@ -2634,10 +2635,10 @@
     </row>
     <row r="53" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>4</v>
@@ -2657,10 +2658,10 @@
     </row>
     <row r="54" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>110</v>
@@ -2680,10 +2681,10 @@
     </row>
     <row r="55" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>21</v>
@@ -2703,10 +2704,10 @@
     </row>
     <row r="56" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>21</v>
@@ -2726,10 +2727,10 @@
     </row>
     <row r="57" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>21</v>
@@ -2749,10 +2750,10 @@
     </row>
     <row r="58" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>133</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>21</v>
@@ -2772,10 +2773,10 @@
     </row>
     <row r="59" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>135</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>21</v>
@@ -2787,7 +2788,7 @@
         <v>24</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G59" s="6" t="s">
         <v>18</v>
@@ -2795,10 +2796,10 @@
     </row>
     <row r="60" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>137</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>21</v>
@@ -2818,10 +2819,10 @@
     </row>
     <row r="61" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>139</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>21</v>
@@ -2839,12 +2840,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>10</v>
@@ -2862,12 +2863,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>142</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>143</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>110</v>
@@ -2887,10 +2888,10 @@
     </row>
     <row r="64" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>21</v>
@@ -2910,10 +2911,10 @@
     </row>
     <row r="65" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>147</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>21</v>
@@ -2933,10 +2934,10 @@
     </row>
     <row r="66" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>21</v>
@@ -2956,10 +2957,10 @@
     </row>
     <row r="67" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B67" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>151</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>4</v>
@@ -2979,10 +2980,10 @@
     </row>
     <row r="68" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>21</v>
@@ -3000,12 +3001,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>76</v>
@@ -3025,10 +3026,10 @@
     </row>
     <row r="70" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>21</v>
@@ -3048,10 +3049,10 @@
     </row>
     <row r="71" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>159</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>4</v>
@@ -3071,10 +3072,10 @@
     </row>
     <row r="72" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>161</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>21</v>
@@ -3094,10 +3095,10 @@
     </row>
     <row r="73" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B73" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>163</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>21</v>
@@ -3117,10 +3118,10 @@
     </row>
     <row r="74" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>21</v>
@@ -3138,12 +3139,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B75" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>10</v>
@@ -3161,12 +3162,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B76" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>168</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>110</v>
@@ -3186,10 +3187,10 @@
     </row>
     <row r="77" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B77" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>170</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>21</v>
@@ -3209,10 +3210,10 @@
     </row>
     <row r="78" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B78" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>172</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>21</v>
@@ -3232,10 +3233,10 @@
     </row>
     <row r="79" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B79" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>174</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>21</v>
@@ -3255,10 +3256,10 @@
     </row>
     <row r="80" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>21</v>
@@ -3278,10 +3279,10 @@
     </row>
     <row r="81" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B81" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>21</v>
@@ -3301,10 +3302,10 @@
     </row>
     <row r="82" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B82" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>35</v>
@@ -3324,10 +3325,10 @@
     </row>
     <row r="83" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B83" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>181</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>21</v>
@@ -3347,10 +3348,10 @@
     </row>
     <row r="84" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>183</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>21</v>
@@ -3370,10 +3371,10 @@
     </row>
     <row r="85" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B85" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>21</v>
@@ -3393,10 +3394,10 @@
     </row>
     <row r="86" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B86" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>21</v>
@@ -3416,10 +3417,10 @@
     </row>
     <row r="87" spans="1:18" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B87" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>21</v>
@@ -3431,7 +3432,7 @@
         <v>24</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G87" s="6" t="s">
         <v>12</v>
@@ -3439,10 +3440,10 @@
     </row>
     <row r="88" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B88" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>4</v>
@@ -3451,7 +3452,7 @@
         <v>3.32</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>6</v>
@@ -3462,19 +3463,19 @@
     </row>
     <row r="89" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>6</v>
@@ -3485,19 +3486,19 @@
     </row>
     <row r="90" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>6</v>
@@ -3508,19 +3509,19 @@
     </row>
     <row r="91" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F91" s="6" t="s">
         <v>6</v>
@@ -3531,19 +3532,19 @@
     </row>
     <row r="92" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>6</v>
@@ -3552,24 +3553,24 @@
         <v>12</v>
       </c>
       <c r="R92" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="93" spans="1:18" ht="51" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>6</v>
@@ -3580,10 +3581,10 @@
     </row>
     <row r="94" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B94" s="6" t="s">
         <v>199</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>200</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>21</v>
@@ -3603,10 +3604,10 @@
     </row>
     <row r="95" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B95" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>21</v>
@@ -3626,10 +3627,10 @@
     </row>
     <row r="96" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B96" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>204</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>35</v>
@@ -3649,10 +3650,10 @@
     </row>
     <row r="97" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B97" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>206</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>21</v>
@@ -3672,10 +3673,10 @@
     </row>
     <row r="98" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B98" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>208</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>21</v>
@@ -3695,10 +3696,10 @@
     </row>
     <row r="99" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>21</v>
@@ -3718,10 +3719,10 @@
     </row>
     <row r="100" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B100" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>211</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>21</v>
@@ -3741,10 +3742,10 @@
     </row>
     <row r="101" spans="1:25" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B101" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>21</v>
@@ -3756,7 +3757,7 @@
         <v>24</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G101" s="6" t="s">
         <v>18</v>
@@ -3764,10 +3765,10 @@
     </row>
     <row r="102" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B102" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>4</v>
@@ -3787,13 +3788,13 @@
     </row>
     <row r="103" spans="1:25" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B103" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B103" s="6" t="s">
+      <c r="C103" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="D103" s="7">
         <v>42.5</v>
@@ -3810,10 +3811,10 @@
     </row>
     <row r="104" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>76</v>
@@ -3831,12 +3832,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B105" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>10</v>
@@ -3856,10 +3857,10 @@
     </row>
     <row r="106" spans="1:25" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B106" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>21</v>
@@ -3871,21 +3872,21 @@
         <v>24</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G106" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Y106" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="107" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B107" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>226</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>21</v>
@@ -3905,10 +3906,10 @@
     </row>
     <row r="108" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B108" s="6" t="s">
         <v>227</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>228</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>4</v>
@@ -3917,7 +3918,7 @@
         <v>22.7</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F108" s="6" t="s">
         <v>6</v>
@@ -3928,10 +3929,10 @@
     </row>
     <row r="109" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B109" s="6" t="s">
         <v>229</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>230</v>
       </c>
       <c r="C109" s="6" t="s">
         <v>21</v>
@@ -3951,10 +3952,10 @@
     </row>
     <row r="110" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B110" s="6" t="s">
         <v>231</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>232</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>4</v>
@@ -3974,10 +3975,10 @@
     </row>
     <row r="111" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B111" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>234</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>21</v>
@@ -3995,12 +3996,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:25" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B112" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>236</v>
       </c>
       <c r="C112" s="6" t="s">
         <v>110</v>
@@ -4020,10 +4021,10 @@
     </row>
     <row r="113" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B113" s="11" t="s">
         <v>251</v>
-      </c>
-      <c r="B113" s="11" t="s">
-        <v>252</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>21</v>
@@ -4043,10 +4044,10 @@
     </row>
     <row r="114" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B114" s="11" t="s">
         <v>253</v>
-      </c>
-      <c r="B114" s="11" t="s">
-        <v>254</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>21</v>
@@ -4064,12 +4065,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B115" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>76</v>
@@ -4087,15 +4088,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B116" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="B116" s="6" t="s">
+      <c r="C116" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>259</v>
       </c>
       <c r="D116" s="7">
         <v>83.8</v>
@@ -4112,10 +4113,10 @@
     </row>
     <row r="117" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="B117" s="11" t="s">
         <v>260</v>
-      </c>
-      <c r="B117" s="11" t="s">
-        <v>261</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>21</v>
@@ -4127,7 +4128,7 @@
         <v>24</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G117" s="6" t="s">
         <v>12</v>
@@ -4135,10 +4136,10 @@
     </row>
     <row r="118" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B118" s="11" t="s">
         <v>263</v>
-      </c>
-      <c r="B118" s="11" t="s">
-        <v>264</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>21</v>
@@ -4158,10 +4159,10 @@
     </row>
     <row r="119" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B119" s="6" t="s">
         <v>265</v>
-      </c>
-      <c r="B119" s="6" t="s">
-        <v>266</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>21</v>
@@ -4179,12 +4180,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B120" s="12" t="s">
         <v>267</v>
-      </c>
-      <c r="B120" s="12" t="s">
-        <v>268</v>
       </c>
       <c r="C120" s="12" t="s">
         <v>76</v>
@@ -4209,7 +4210,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4218,7 +4219,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>